<commit_message>
- Chạy project với threshold = 160 - Tạo chart cho các bảng thực nghiệm
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
   </bookViews>
   <sheets>
     <sheet name="Threshold=123" sheetId="1" r:id="rId1"/>
     <sheet name="Threshold=40" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Threshold=160" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="21">
   <si>
     <t>Lần 1</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Thực nghiệm thực hiện với threshold = 40</t>
+  </si>
+  <si>
+    <t>Thực nghiệm thực hiện với threshold = 160</t>
   </si>
 </sst>
 </file>
@@ -205,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -226,18 +229,19 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -252,6 +256,987 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Thực Nghiệm 50-50</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Threshold=123'!$B$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0%">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0%">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0%">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0%">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0%">
+                  <c:v>0.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="84547456"/>
+        <c:axId val="84548992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="84547456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84548992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84548992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84547456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Thực Nghiệm K-folds</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Threshold=123'!$B$18:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.59160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68235000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75312500000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86785000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86919999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85829999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.88636000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0%">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89439999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="54671232"/>
+        <c:axId val="54672768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="54671232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54672768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="54672768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54671232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Thực Nghiệm 50-50</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Threshold=40'!$B$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.495</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="84972288"/>
+        <c:axId val="84973824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="84972288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84973824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84973824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="84972288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Thực Nghiệm K-folds</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Threshold=40'!$B$18:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.18611111111111112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2411764705882353</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.43214285714285716</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.43461538461538463</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.47916666666666669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42727272727272725</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51666666666666672</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="54659712"/>
+        <c:axId val="55698944"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="54659712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55698944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="55698944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54659712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Thực Nghiệm K-folds</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Threshold=160'!$B$18:$K$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.59166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68235294117647061</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75312500000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86785714285714288</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.86923076923076925</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85833333333333328</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.88636363636363635</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89444444444444449</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="83613184"/>
+        <c:axId val="83614720"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="83613184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83614720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="83614720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83613184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Thực Nghiệm 50-50</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Threshold=160'!$B$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="83968384"/>
+        <c:axId val="83969920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="83968384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83969920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="83969920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83968384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -543,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,31 +1538,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -615,7 +1600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -791,16 +1776,16 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -1011,17 +1996,17 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1031,6 +2016,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1038,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,25 +2034,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -1290,16 +2276,16 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -1539,17 +2525,515 @@
     <mergeCell ref="A12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <v>200</v>
+      </c>
+      <c r="C5" s="4">
+        <v>200</v>
+      </c>
+      <c r="D5" s="4">
+        <v>200</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" s="4">
+        <v>200</v>
+      </c>
+      <c r="G5" s="4">
+        <v>200</v>
+      </c>
+      <c r="H5" s="4">
+        <v>200</v>
+      </c>
+      <c r="I5" s="4">
+        <v>200</v>
+      </c>
+      <c r="J5" s="4">
+        <v>200</v>
+      </c>
+      <c r="K5" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4">
+        <v>200</v>
+      </c>
+      <c r="C6" s="4">
+        <v>200</v>
+      </c>
+      <c r="D6" s="4">
+        <v>200</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" s="4">
+        <v>200</v>
+      </c>
+      <c r="G6" s="4">
+        <v>200</v>
+      </c>
+      <c r="H6" s="4">
+        <v>200</v>
+      </c>
+      <c r="I6" s="4">
+        <v>200</v>
+      </c>
+      <c r="J6" s="4">
+        <v>200</v>
+      </c>
+      <c r="K6" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>176</v>
+      </c>
+      <c r="C7" s="4">
+        <v>177</v>
+      </c>
+      <c r="D7" s="4">
+        <v>188</v>
+      </c>
+      <c r="E7" s="4">
+        <v>184</v>
+      </c>
+      <c r="F7" s="4">
+        <v>176</v>
+      </c>
+      <c r="G7" s="4">
+        <v>178</v>
+      </c>
+      <c r="H7" s="4">
+        <v>183</v>
+      </c>
+      <c r="I7" s="4">
+        <v>180</v>
+      </c>
+      <c r="J7" s="4">
+        <v>187</v>
+      </c>
+      <c r="K7" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4">
+        <v>36</v>
+      </c>
+      <c r="D8" s="4">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4">
+        <v>35</v>
+      </c>
+      <c r="G8" s="4">
+        <v>36</v>
+      </c>
+      <c r="H8" s="4">
+        <v>35</v>
+      </c>
+      <c r="I8" s="4">
+        <v>37</v>
+      </c>
+      <c r="J8" s="4">
+        <v>37</v>
+      </c>
+      <c r="K8" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5">
+        <f>B7/B6</f>
+        <v>0.88</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" ref="C9:J9" si="0">C7/C6</f>
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.89</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" ref="K9" si="1">ROUND((K7/K6),2)</f>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4">
+        <v>80</v>
+      </c>
+      <c r="E14" s="4">
+        <v>100</v>
+      </c>
+      <c r="F14" s="4">
+        <v>120</v>
+      </c>
+      <c r="G14" s="4">
+        <v>140</v>
+      </c>
+      <c r="H14" s="4">
+        <v>160</v>
+      </c>
+      <c r="I14" s="4">
+        <v>180</v>
+      </c>
+      <c r="J14" s="4">
+        <v>200</v>
+      </c>
+      <c r="K14" s="4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>360</v>
+      </c>
+      <c r="C15" s="4">
+        <v>340</v>
+      </c>
+      <c r="D15" s="4">
+        <v>320</v>
+      </c>
+      <c r="E15" s="4">
+        <v>300</v>
+      </c>
+      <c r="F15" s="4">
+        <v>280</v>
+      </c>
+      <c r="G15" s="4">
+        <v>260</v>
+      </c>
+      <c r="H15" s="4">
+        <v>240</v>
+      </c>
+      <c r="I15" s="4">
+        <v>220</v>
+      </c>
+      <c r="J15" s="4">
+        <v>200</v>
+      </c>
+      <c r="K15" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>213</v>
+      </c>
+      <c r="C16" s="4">
+        <v>232</v>
+      </c>
+      <c r="D16" s="4">
+        <v>241</v>
+      </c>
+      <c r="E16" s="4">
+        <v>239</v>
+      </c>
+      <c r="F16" s="4">
+        <v>243</v>
+      </c>
+      <c r="G16" s="4">
+        <v>226</v>
+      </c>
+      <c r="H16" s="4">
+        <v>206</v>
+      </c>
+      <c r="I16" s="4">
+        <v>195</v>
+      </c>
+      <c r="J16" s="4">
+        <v>178</v>
+      </c>
+      <c r="K16" s="4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <v>32</v>
+      </c>
+      <c r="C17" s="4">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4">
+        <v>34</v>
+      </c>
+      <c r="E17" s="4">
+        <v>35</v>
+      </c>
+      <c r="F17" s="4">
+        <v>35</v>
+      </c>
+      <c r="G17" s="4">
+        <v>35</v>
+      </c>
+      <c r="H17" s="4">
+        <v>35</v>
+      </c>
+      <c r="I17" s="4">
+        <v>35</v>
+      </c>
+      <c r="J17" s="4">
+        <v>35</v>
+      </c>
+      <c r="K17" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B16/B15</f>
+        <v>0.59166666666666667</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" ref="C18:K18" si="2">C16/C15</f>
+        <v>0.68235294117647061</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.75312500000000004</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.79666666666666663</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.86785714285714288</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.86923076923076925</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.85833333333333328</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.88636363636363635</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.89</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.89444444444444449</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A12:H12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Báo cáo: xóa bảng cũ, thêm mục mô tả chương trình (chưa viết). - Ststistic: chỉnh sửa tất cả chart cho đồng nhất với nhau. - Slide: chỉnh sửa slide đầu, điều chỉnh 1 slide bị lệch trái, chuyển sang pptx.
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LBP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Threshold=123" sheetId="1" r:id="rId1"/>
-    <sheet name="Threshold=40" sheetId="2" r:id="rId2"/>
+    <sheet name="Threshold=40" sheetId="2" r:id="rId1"/>
+    <sheet name="Threshold=123" sheetId="1" r:id="rId2"/>
     <sheet name="Threshold=160" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -254,6 +259,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -290,41 +298,63 @@
             <c:v>Thực Nghiệm 50-50</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Threshold=123'!$B$9:$K$9</c:f>
+              <c:f>'Threshold=40'!$B$9:$K$9</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0" formatCode="0%">
-                  <c:v>0.88</c:v>
+                <c:pt idx="0">
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0%">
-                  <c:v>0.92</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0%">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0%">
-                  <c:v>0.89</c:v>
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.91500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0%">
-                  <c:v>0.9</c:v>
+                  <c:v>0.495</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.93500000000000005</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0%">
-                  <c:v>0.91</c:v>
+                  <c:v>0.54500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -339,11 +369,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="84547456"/>
-        <c:axId val="84548992"/>
+        <c:axId val="171666008"/>
+        <c:axId val="171668440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84547456"/>
+        <c:axId val="171666008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -352,7 +382,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84548992"/>
+        <c:crossAx val="171668440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -360,9 +390,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84548992"/>
+        <c:axId val="171668440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -371,7 +402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84547456"/>
+        <c:crossAx val="171666008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -420,41 +451,63 @@
             <c:v>Thực Nghiệm K-folds</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Threshold=123'!$B$18:$K$18</c:f>
+              <c:f>'Threshold=40'!$B$18:$K$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.59160000000000001</c:v>
+                  <c:v>0.18611111111111112</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.68235000000000001</c:v>
+                  <c:v>0.2411764705882353</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75312500000000004</c:v>
+                  <c:v>0.28125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79659999999999997</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86785000000000001</c:v>
+                  <c:v>0.43214285714285716</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.86919999999999997</c:v>
+                  <c:v>0.43461538461538463</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.85829999999999995</c:v>
+                  <c:v>0.47916666666666669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.88636000000000004</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0%">
-                  <c:v>0.89</c:v>
+                  <c:v>0.42727272727272725</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.89439999999999997</c:v>
+                  <c:v>0.51666666666666672</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -469,11 +522,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="54671232"/>
-        <c:axId val="54672768"/>
+        <c:axId val="170774512"/>
+        <c:axId val="170774904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54671232"/>
+        <c:axId val="170774512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,7 +535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54672768"/>
+        <c:crossAx val="170774904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -490,18 +543,19 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54672768"/>
+        <c:axId val="170774904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54671232"/>
+        <c:crossAx val="170774512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -550,41 +604,63 @@
             <c:v>Thực Nghiệm 50-50</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Threshold=40'!$B$9:$K$9</c:f>
+              <c:f>'Threshold=123'!$B$9:$K$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.38</c:v>
+                <c:pt idx="0" formatCode="0%">
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.54500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.45500000000000002</c:v>
+                  <c:v>0.88500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0%">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0%">
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.495</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.53</c:v>
+                  <c:v>0.91500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0%">
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.54500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.52</c:v>
+                  <c:v>0.93500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0%">
+                  <c:v>0.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,11 +675,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="84972288"/>
-        <c:axId val="84973824"/>
+        <c:axId val="171506072"/>
+        <c:axId val="171506456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84972288"/>
+        <c:axId val="171506072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84973824"/>
+        <c:crossAx val="171506456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,9 +696,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84973824"/>
+        <c:axId val="171506456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -631,7 +709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84972288"/>
+        <c:crossAx val="171506072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -680,41 +758,63 @@
             <c:v>Thực Nghiệm K-folds</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Threshold=40'!$B$18:$K$18</c:f>
+              <c:f>'Threshold=123'!$B$18:$K$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.18611111111111112</c:v>
+                  <c:v>0.59160000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2411764705882353</c:v>
+                  <c:v>0.68235000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28125</c:v>
+                  <c:v>0.75312500000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.37</c:v>
+                  <c:v>0.79659999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43214285714285716</c:v>
+                  <c:v>0.86785000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.43461538461538463</c:v>
+                  <c:v>0.86919999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47916666666666669</c:v>
+                  <c:v>0.85829999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.42727272727272725</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.45</c:v>
+                  <c:v>0.88636000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0%">
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.51666666666666672</c:v>
+                  <c:v>0.89439999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,11 +829,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="54659712"/>
-        <c:axId val="55698944"/>
+        <c:axId val="172055720"/>
+        <c:axId val="172056104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54659712"/>
+        <c:axId val="172055720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,7 +842,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55698944"/>
+        <c:crossAx val="172056104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -750,18 +850,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55698944"/>
+        <c:axId val="172056104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54659712"/>
+        <c:crossAx val="172055720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -810,6 +910,28 @@
             <c:v>Thực Nghiệm K-folds</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'Threshold=160'!$B$18:$K$18</c:f>
@@ -859,11 +981,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="83613184"/>
-        <c:axId val="83614720"/>
+        <c:axId val="170775688"/>
+        <c:axId val="170776080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83613184"/>
+        <c:axId val="170775688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,7 +994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83614720"/>
+        <c:crossAx val="170776080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -880,18 +1002,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83614720"/>
+        <c:axId val="170776080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83613184"/>
+        <c:crossAx val="170775688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -940,6 +1062,28 @@
             <c:v>Thực Nghiệm 50-50</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'Threshold=160'!$B$9:$K$9</c:f>
@@ -989,11 +1133,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="83968384"/>
-        <c:axId val="83969920"/>
+        <c:axId val="172061392"/>
+        <c:axId val="172061784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83968384"/>
+        <c:axId val="172061392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1146,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83969920"/>
+        <c:crossAx val="172061784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,9 +1154,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83969920"/>
+        <c:axId val="172061784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1021,7 +1167,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83968384"/>
+        <c:crossAx val="172061392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1043,15 +1189,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1072,20 +1218,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1110,15 +1256,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1139,20 +1285,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1176,16 +1322,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1207,15 +1353,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1282,7 +1428,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1317,7 +1463,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1528,8 +1674,517 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <v>200</v>
+      </c>
+      <c r="C5" s="4">
+        <v>200</v>
+      </c>
+      <c r="D5" s="4">
+        <v>200</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" s="4">
+        <v>200</v>
+      </c>
+      <c r="G5" s="4">
+        <v>200</v>
+      </c>
+      <c r="H5" s="4">
+        <v>200</v>
+      </c>
+      <c r="I5" s="4">
+        <v>200</v>
+      </c>
+      <c r="J5" s="4">
+        <v>200</v>
+      </c>
+      <c r="K5" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4">
+        <v>200</v>
+      </c>
+      <c r="C6" s="4">
+        <v>200</v>
+      </c>
+      <c r="D6" s="4">
+        <v>200</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" s="4">
+        <v>200</v>
+      </c>
+      <c r="G6" s="4">
+        <v>200</v>
+      </c>
+      <c r="H6" s="4">
+        <v>200</v>
+      </c>
+      <c r="I6" s="4">
+        <v>200</v>
+      </c>
+      <c r="J6" s="4">
+        <v>200</v>
+      </c>
+      <c r="K6" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>76</v>
+      </c>
+      <c r="C7" s="4">
+        <v>92</v>
+      </c>
+      <c r="D7" s="4">
+        <v>112</v>
+      </c>
+      <c r="E7" s="4">
+        <v>109</v>
+      </c>
+      <c r="F7" s="4">
+        <v>90</v>
+      </c>
+      <c r="G7" s="4">
+        <v>91</v>
+      </c>
+      <c r="H7" s="4">
+        <v>99</v>
+      </c>
+      <c r="I7" s="4">
+        <v>106</v>
+      </c>
+      <c r="J7" s="4">
+        <v>109</v>
+      </c>
+      <c r="K7" s="4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4">
+        <v>24</v>
+      </c>
+      <c r="G8" s="4">
+        <v>23</v>
+      </c>
+      <c r="H8" s="4">
+        <v>23</v>
+      </c>
+      <c r="I8" s="4">
+        <v>23</v>
+      </c>
+      <c r="J8" s="4">
+        <v>23</v>
+      </c>
+      <c r="K8" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5">
+        <f>B7/B6</f>
+        <v>0.38</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" ref="C9:J9" si="0">C7/C6</f>
+        <v>0.46</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.495</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" ref="K9" si="1">ROUND((K7/K6),2)</f>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4">
+        <v>80</v>
+      </c>
+      <c r="E14" s="4">
+        <v>100</v>
+      </c>
+      <c r="F14" s="4">
+        <v>120</v>
+      </c>
+      <c r="G14" s="4">
+        <v>140</v>
+      </c>
+      <c r="H14" s="4">
+        <v>160</v>
+      </c>
+      <c r="I14" s="4">
+        <v>180</v>
+      </c>
+      <c r="J14" s="4">
+        <v>200</v>
+      </c>
+      <c r="K14" s="4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>360</v>
+      </c>
+      <c r="C15" s="4">
+        <v>340</v>
+      </c>
+      <c r="D15" s="4">
+        <v>320</v>
+      </c>
+      <c r="E15" s="4">
+        <v>300</v>
+      </c>
+      <c r="F15" s="4">
+        <v>280</v>
+      </c>
+      <c r="G15" s="4">
+        <v>260</v>
+      </c>
+      <c r="H15" s="4">
+        <v>240</v>
+      </c>
+      <c r="I15" s="4">
+        <v>220</v>
+      </c>
+      <c r="J15" s="4">
+        <v>200</v>
+      </c>
+      <c r="K15" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>67</v>
+      </c>
+      <c r="C16" s="4">
+        <v>82</v>
+      </c>
+      <c r="D16" s="4">
+        <v>90</v>
+      </c>
+      <c r="E16" s="4">
+        <v>111</v>
+      </c>
+      <c r="F16" s="4">
+        <v>121</v>
+      </c>
+      <c r="G16" s="4">
+        <v>113</v>
+      </c>
+      <c r="H16" s="4">
+        <v>115</v>
+      </c>
+      <c r="I16" s="4">
+        <v>94</v>
+      </c>
+      <c r="J16" s="4">
+        <v>90</v>
+      </c>
+      <c r="K16" s="4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4">
+        <v>21</v>
+      </c>
+      <c r="D17" s="4">
+        <v>22</v>
+      </c>
+      <c r="E17" s="4">
+        <v>23</v>
+      </c>
+      <c r="F17" s="4">
+        <v>22</v>
+      </c>
+      <c r="G17" s="4">
+        <v>23</v>
+      </c>
+      <c r="H17" s="4">
+        <v>23</v>
+      </c>
+      <c r="I17" s="4">
+        <v>23</v>
+      </c>
+      <c r="J17" s="4">
+        <v>23</v>
+      </c>
+      <c r="K17" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B16/B15</f>
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" ref="C18:K18" si="2">C16/C15</f>
+        <v>0.2411764705882353</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.28125</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.37</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.43214285714285716</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.43461538461538463</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.42727272727272725</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.51666666666666672</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A12:H12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,12 +2675,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,7 +2690,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -2053,9 +2708,9 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -2165,34 +2820,34 @@
         <v>12</v>
       </c>
       <c r="B7" s="4">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="C7" s="4">
-        <v>92</v>
+        <v>177</v>
       </c>
       <c r="D7" s="4">
-        <v>112</v>
+        <v>188</v>
       </c>
       <c r="E7" s="4">
-        <v>109</v>
+        <v>184</v>
       </c>
       <c r="F7" s="4">
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="G7" s="4">
-        <v>91</v>
+        <v>178</v>
       </c>
       <c r="H7" s="4">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="I7" s="4">
-        <v>106</v>
+        <v>180</v>
       </c>
       <c r="J7" s="4">
-        <v>109</v>
+        <v>187</v>
       </c>
       <c r="K7" s="4">
-        <v>103</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2200,34 +2855,34 @@
         <v>18</v>
       </c>
       <c r="B8" s="4">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C8" s="4">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D8" s="4">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E8" s="4">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G8" s="4">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="H8" s="4">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="I8" s="4">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="J8" s="4">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K8" s="4">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2236,43 +2891,43 @@
       </c>
       <c r="B9" s="5">
         <f>B7/B6</f>
-        <v>0.38</v>
+        <v>0.88</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" ref="C9:J9" si="0">C7/C6</f>
-        <v>0.46</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.94</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>0.54500000000000004</v>
+        <v>0.92</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>0.45</v>
+        <v>0.88</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>0.45500000000000002</v>
+        <v>0.89</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="0"/>
-        <v>0.495</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="0"/>
-        <v>0.53</v>
+        <v>0.9</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="0"/>
-        <v>0.54500000000000004</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ref="K9" si="1">ROUND((K7/K6),2)</f>
-        <v>0.52</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2395,34 +3050,34 @@
         <v>12</v>
       </c>
       <c r="B16" s="4">
-        <v>67</v>
+        <v>213</v>
       </c>
       <c r="C16" s="4">
-        <v>82</v>
+        <v>232</v>
       </c>
       <c r="D16" s="4">
-        <v>90</v>
+        <v>241</v>
       </c>
       <c r="E16" s="4">
-        <v>111</v>
+        <v>239</v>
       </c>
       <c r="F16" s="4">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="G16" s="4">
-        <v>113</v>
+        <v>226</v>
       </c>
       <c r="H16" s="4">
-        <v>115</v>
+        <v>206</v>
       </c>
       <c r="I16" s="4">
-        <v>94</v>
+        <v>195</v>
       </c>
       <c r="J16" s="4">
-        <v>90</v>
+        <v>178</v>
       </c>
       <c r="K16" s="4">
-        <v>93</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2430,34 +3085,34 @@
         <v>13</v>
       </c>
       <c r="B17" s="4">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D17" s="4">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E17" s="4">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F17" s="4">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G17" s="4">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H17" s="4">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="I17" s="4">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="J17" s="4">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="K17" s="4">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2466,43 +3121,43 @@
       </c>
       <c r="B18" s="6">
         <f>B16/B15</f>
-        <v>0.18611111111111112</v>
+        <v>0.59166666666666667</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" ref="C18:K18" si="2">C16/C15</f>
-        <v>0.2411764705882353</v>
+        <v>0.68235294117647061</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="2"/>
-        <v>0.28125</v>
+        <v>0.75312500000000004</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="2"/>
-        <v>0.37</v>
+        <v>0.79666666666666663</v>
       </c>
       <c r="F18" s="6">
         <f t="shared" si="2"/>
-        <v>0.43214285714285716</v>
+        <v>0.86785714285714288</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" si="2"/>
-        <v>0.43461538461538463</v>
+        <v>0.86923076923076925</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" si="2"/>
-        <v>0.47916666666666669</v>
+        <v>0.85833333333333328</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" si="2"/>
-        <v>0.42727272727272725</v>
+        <v>0.88636363636363635</v>
       </c>
       <c r="J18" s="6">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.89</v>
       </c>
       <c r="K18" s="6">
         <f t="shared" si="2"/>
-        <v>0.51666666666666672</v>
+        <v>0.89444444444444449</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2527,513 +3182,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
-  <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4">
-        <v>200</v>
-      </c>
-      <c r="C5" s="4">
-        <v>200</v>
-      </c>
-      <c r="D5" s="4">
-        <v>200</v>
-      </c>
-      <c r="E5" s="4">
-        <v>200</v>
-      </c>
-      <c r="F5" s="4">
-        <v>200</v>
-      </c>
-      <c r="G5" s="4">
-        <v>200</v>
-      </c>
-      <c r="H5" s="4">
-        <v>200</v>
-      </c>
-      <c r="I5" s="4">
-        <v>200</v>
-      </c>
-      <c r="J5" s="4">
-        <v>200</v>
-      </c>
-      <c r="K5" s="4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4">
-        <v>200</v>
-      </c>
-      <c r="C6" s="4">
-        <v>200</v>
-      </c>
-      <c r="D6" s="4">
-        <v>200</v>
-      </c>
-      <c r="E6" s="4">
-        <v>200</v>
-      </c>
-      <c r="F6" s="4">
-        <v>200</v>
-      </c>
-      <c r="G6" s="4">
-        <v>200</v>
-      </c>
-      <c r="H6" s="4">
-        <v>200</v>
-      </c>
-      <c r="I6" s="4">
-        <v>200</v>
-      </c>
-      <c r="J6" s="4">
-        <v>200</v>
-      </c>
-      <c r="K6" s="4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4">
-        <v>176</v>
-      </c>
-      <c r="C7" s="4">
-        <v>177</v>
-      </c>
-      <c r="D7" s="4">
-        <v>188</v>
-      </c>
-      <c r="E7" s="4">
-        <v>184</v>
-      </c>
-      <c r="F7" s="4">
-        <v>176</v>
-      </c>
-      <c r="G7" s="4">
-        <v>178</v>
-      </c>
-      <c r="H7" s="4">
-        <v>183</v>
-      </c>
-      <c r="I7" s="4">
-        <v>180</v>
-      </c>
-      <c r="J7" s="4">
-        <v>187</v>
-      </c>
-      <c r="K7" s="4">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4">
-        <v>37</v>
-      </c>
-      <c r="C8" s="4">
-        <v>36</v>
-      </c>
-      <c r="D8" s="4">
-        <v>36</v>
-      </c>
-      <c r="E8" s="4">
-        <v>36</v>
-      </c>
-      <c r="F8" s="4">
-        <v>35</v>
-      </c>
-      <c r="G8" s="4">
-        <v>36</v>
-      </c>
-      <c r="H8" s="4">
-        <v>35</v>
-      </c>
-      <c r="I8" s="4">
-        <v>37</v>
-      </c>
-      <c r="J8" s="4">
-        <v>37</v>
-      </c>
-      <c r="K8" s="4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5">
-        <f>B7/B6</f>
-        <v>0.88</v>
-      </c>
-      <c r="C9" s="5">
-        <f t="shared" ref="C9:J9" si="0">C7/C6</f>
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="D9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.94</v>
-      </c>
-      <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-      <c r="F9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.88</v>
-      </c>
-      <c r="G9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.89</v>
-      </c>
-      <c r="H9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="I9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.9</v>
-      </c>
-      <c r="J9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="K9" s="5">
-        <f t="shared" ref="K9" si="1">ROUND((K7/K6),2)</f>
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4">
-        <v>40</v>
-      </c>
-      <c r="C14" s="4">
-        <v>60</v>
-      </c>
-      <c r="D14" s="4">
-        <v>80</v>
-      </c>
-      <c r="E14" s="4">
-        <v>100</v>
-      </c>
-      <c r="F14" s="4">
-        <v>120</v>
-      </c>
-      <c r="G14" s="4">
-        <v>140</v>
-      </c>
-      <c r="H14" s="4">
-        <v>160</v>
-      </c>
-      <c r="I14" s="4">
-        <v>180</v>
-      </c>
-      <c r="J14" s="4">
-        <v>200</v>
-      </c>
-      <c r="K14" s="4">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4">
-        <v>360</v>
-      </c>
-      <c r="C15" s="4">
-        <v>340</v>
-      </c>
-      <c r="D15" s="4">
-        <v>320</v>
-      </c>
-      <c r="E15" s="4">
-        <v>300</v>
-      </c>
-      <c r="F15" s="4">
-        <v>280</v>
-      </c>
-      <c r="G15" s="4">
-        <v>260</v>
-      </c>
-      <c r="H15" s="4">
-        <v>240</v>
-      </c>
-      <c r="I15" s="4">
-        <v>220</v>
-      </c>
-      <c r="J15" s="4">
-        <v>200</v>
-      </c>
-      <c r="K15" s="4">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="4">
-        <v>213</v>
-      </c>
-      <c r="C16" s="4">
-        <v>232</v>
-      </c>
-      <c r="D16" s="4">
-        <v>241</v>
-      </c>
-      <c r="E16" s="4">
-        <v>239</v>
-      </c>
-      <c r="F16" s="4">
-        <v>243</v>
-      </c>
-      <c r="G16" s="4">
-        <v>226</v>
-      </c>
-      <c r="H16" s="4">
-        <v>206</v>
-      </c>
-      <c r="I16" s="4">
-        <v>195</v>
-      </c>
-      <c r="J16" s="4">
-        <v>178</v>
-      </c>
-      <c r="K16" s="4">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4">
-        <v>32</v>
-      </c>
-      <c r="C17" s="4">
-        <v>33</v>
-      </c>
-      <c r="D17" s="4">
-        <v>34</v>
-      </c>
-      <c r="E17" s="4">
-        <v>35</v>
-      </c>
-      <c r="F17" s="4">
-        <v>35</v>
-      </c>
-      <c r="G17" s="4">
-        <v>35</v>
-      </c>
-      <c r="H17" s="4">
-        <v>35</v>
-      </c>
-      <c r="I17" s="4">
-        <v>35</v>
-      </c>
-      <c r="J17" s="4">
-        <v>35</v>
-      </c>
-      <c r="K17" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="6">
-        <f>B16/B15</f>
-        <v>0.59166666666666667</v>
-      </c>
-      <c r="C18" s="6">
-        <f t="shared" ref="C18:K18" si="2">C16/C15</f>
-        <v>0.68235294117647061</v>
-      </c>
-      <c r="D18" s="6">
-        <f t="shared" si="2"/>
-        <v>0.75312500000000004</v>
-      </c>
-      <c r="E18" s="6">
-        <f t="shared" si="2"/>
-        <v>0.79666666666666663</v>
-      </c>
-      <c r="F18" s="6">
-        <f t="shared" si="2"/>
-        <v>0.86785714285714288</v>
-      </c>
-      <c r="G18" s="6">
-        <f t="shared" si="2"/>
-        <v>0.86923076923076925</v>
-      </c>
-      <c r="H18" s="6">
-        <f t="shared" si="2"/>
-        <v>0.85833333333333328</v>
-      </c>
-      <c r="I18" s="6">
-        <f t="shared" si="2"/>
-        <v>0.88636363636363635</v>
-      </c>
-      <c r="J18" s="6">
-        <f t="shared" si="2"/>
-        <v>0.89</v>
-      </c>
-      <c r="K18" s="6">
-        <f t="shared" si="2"/>
-        <v>0.89444444444444449</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A12:H12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- Thống kê thêm phần so sánh các phương pháp, bổ sung vào báo cáo. - Chỉnh sửa slide.
</commit_message>
<xml_diff>
--- a/Statistic.xlsx
+++ b/Statistic.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Threshold=40" sheetId="2" r:id="rId1"/>
     <sheet name="Threshold=123" sheetId="1" r:id="rId2"/>
     <sheet name="Threshold=160" sheetId="3" r:id="rId3"/>
+    <sheet name="AT&amp;T" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="27">
   <si>
     <t>Lần 1</t>
   </si>
@@ -85,11 +86,32 @@
   <si>
     <t>Thực nghiệm thực hiện với threshold = 160</t>
   </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>ICA</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>HGPP</t>
+  </si>
+  <si>
+    <t>LBP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -181,39 +203,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -235,12 +229,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -248,7 +238,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -281,7 +270,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -315,7 +303,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -369,11 +356,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171666008"/>
-        <c:axId val="171668440"/>
+        <c:axId val="184952808"/>
+        <c:axId val="184961384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171666008"/>
+        <c:axId val="184952808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -382,7 +369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171668440"/>
+        <c:crossAx val="184961384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -390,7 +377,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171668440"/>
+        <c:axId val="184961384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -402,7 +389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171666008"/>
+        <c:crossAx val="184952808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -434,7 +421,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -468,7 +454,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -522,11 +507,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170774512"/>
-        <c:axId val="170774904"/>
+        <c:axId val="185088856"/>
+        <c:axId val="185093336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170774512"/>
+        <c:axId val="185088856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +520,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170774904"/>
+        <c:crossAx val="185093336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +528,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170774904"/>
+        <c:axId val="185093336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -555,7 +540,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170774512"/>
+        <c:crossAx val="185088856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -675,11 +660,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171506072"/>
-        <c:axId val="171506456"/>
+        <c:axId val="184857536"/>
+        <c:axId val="184844880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171506072"/>
+        <c:axId val="184857536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171506456"/>
+        <c:crossAx val="184844880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -696,7 +681,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171506456"/>
+        <c:axId val="184844880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -709,7 +694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171506072"/>
+        <c:crossAx val="184857536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -829,11 +814,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="172055720"/>
-        <c:axId val="172056104"/>
+        <c:axId val="183811088"/>
+        <c:axId val="183811480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172055720"/>
+        <c:axId val="183811088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172056104"/>
+        <c:crossAx val="183811480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -850,7 +835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172056104"/>
+        <c:axId val="183811480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172055720"/>
+        <c:crossAx val="183811088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -893,7 +878,158 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Thực Nghiệm 50-50</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Threshold=160'!$B$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="185175904"/>
+        <c:axId val="185176296"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="185175904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="185176296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="185176296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="185175904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -927,7 +1063,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -981,11 +1116,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170775688"/>
-        <c:axId val="170776080"/>
+        <c:axId val="185175120"/>
+        <c:axId val="185177080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170775688"/>
+        <c:axId val="185175120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,7 +1129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170776080"/>
+        <c:crossAx val="185177080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1002,7 +1137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170776080"/>
+        <c:axId val="185177080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,7 +1148,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170775688"/>
+        <c:crossAx val="185175120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1030,7 +1165,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1045,8 +1180,65 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Độ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> chính xác (%) ATT</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1059,8 +1251,25 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Thực Nghiệm 50-50</c:v>
+            <c:strRef>
+              <c:f>'AT&amp;T'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
@@ -1070,6 +1279,28 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1081,44 +1312,506 @@
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Threshold=160'!$B$9:$K$9</c:f>
+              <c:f>'AT&amp;T'!$B$2</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.88500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.92</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.89</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.91500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.93500000000000005</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.91</c:v>
+                  <c:v>0.80897849999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AT&amp;T'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PCA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'AT&amp;T'!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.91300000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AT&amp;T'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'AT&amp;T'!$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.94399999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AT&amp;T'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ICA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'AT&amp;T'!$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.91300000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AT&amp;T'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'AT&amp;T'!$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.95599999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AT&amp;T'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HGPP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'AT&amp;T'!$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.98899999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1132,21 +1825,23 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="172061392"/>
-        <c:axId val="172061784"/>
+        <c:gapWidth val="96"/>
+        <c:overlap val="-88"/>
+        <c:axId val="185175512"/>
+        <c:axId val="185177864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172061392"/>
+        <c:axId val="185175512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172061784"/>
+        <c:crossAx val="185177864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1154,7 +1849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172061784"/>
+        <c:axId val="185177864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1162,26 +1857,673 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172061392"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="185175512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1218,20 +2560,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>200024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1294,7 +2636,7 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1322,36 +2664,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -1376,7 +2688,74 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1672,25 +3051,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
@@ -2154,19 +3533,6 @@
         <f t="shared" si="2"/>
         <v>0.51666666666666672</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2181,15 +3547,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2649,19 +4016,6 @@
       <c r="K18" s="6">
         <v>0.89439999999999997</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2677,25 +4031,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
@@ -3160,19 +4514,6 @@
         <v>0.89444444444444449</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
@@ -3182,4 +4523,69 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9">
+        <f>AVERAGE('Threshold=123'!B18:K18)</f>
+        <v>0.80897849999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.98899999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>